<commit_message>
finished the final sweep -- filenames not checked in fastqfiles
</commit_message>
<xml_diff>
--- a/library/library_J.PLAGGENBERG_07.01.19.xlsx
+++ b/library/library_J.PLAGGENBERG_07.01.19.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">GAGTTG</t>
   </si>
   <si>
-    <t xml:space="preserve">E7420</t>
+    <t xml:space="preserve">E7420L</t>
   </si>
   <si>
     <t xml:space="preserve">GCTTAGA</t>
@@ -396,8 +396,8 @@
   </sheetPr>
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:L49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -491,7 +491,8 @@
       <c r="K2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="8" t="b">
+      <c r="L2" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -529,7 +530,8 @@
       <c r="K3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="8" t="b">
+      <c r="L3" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -567,7 +569,8 @@
       <c r="K4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="8" t="b">
+      <c r="L4" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -605,7 +608,8 @@
       <c r="K5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="8" t="b">
+      <c r="L5" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -643,7 +647,8 @@
       <c r="K6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="8" t="b">
+      <c r="L6" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -681,7 +686,8 @@
       <c r="K7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="8" t="b">
+      <c r="L7" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -719,7 +725,8 @@
       <c r="K8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="8" t="b">
+      <c r="L8" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -757,7 +764,8 @@
       <c r="K9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="8" t="b">
+      <c r="L9" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -795,7 +803,8 @@
       <c r="K10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="8" t="b">
+      <c r="L10" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -833,7 +842,8 @@
       <c r="K11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="8" t="b">
+      <c r="L11" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -871,7 +881,8 @@
       <c r="K12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="8" t="b">
+      <c r="L12" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -909,7 +920,8 @@
       <c r="K13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="8" t="b">
+      <c r="L13" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -947,7 +959,8 @@
       <c r="K14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="8" t="b">
+      <c r="L14" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -985,7 +998,8 @@
       <c r="K15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="8" t="b">
+      <c r="L15" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1023,7 +1037,8 @@
       <c r="K16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="8" t="b">
+      <c r="L16" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1061,7 +1076,8 @@
       <c r="K17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="8" t="b">
+      <c r="L17" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1099,7 +1115,8 @@
       <c r="K18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="8" t="b">
+      <c r="L18" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1137,7 +1154,8 @@
       <c r="K19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="8" t="b">
+      <c r="L19" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1175,7 +1193,8 @@
       <c r="K20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="8" t="b">
+      <c r="L20" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1213,7 +1232,8 @@
       <c r="K21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L21" s="8" t="b">
+      <c r="L21" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1251,7 +1271,8 @@
       <c r="K22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="8" t="b">
+      <c r="L22" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1289,7 +1310,8 @@
       <c r="K23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="8" t="b">
+      <c r="L23" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1327,7 +1349,8 @@
       <c r="K24" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="8" t="b">
+      <c r="L24" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1365,7 +1388,8 @@
       <c r="K25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="8" t="b">
+      <c r="L25" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1403,7 +1427,8 @@
       <c r="K26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L26" s="8" t="b">
+      <c r="L26" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1441,7 +1466,8 @@
       <c r="K27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="8" t="b">
+      <c r="L27" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1479,7 +1505,8 @@
       <c r="K28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L28" s="8" t="b">
+      <c r="L28" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1517,7 +1544,8 @@
       <c r="K29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L29" s="8" t="b">
+      <c r="L29" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1555,7 +1583,8 @@
       <c r="K30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L30" s="8" t="b">
+      <c r="L30" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1593,7 +1622,8 @@
       <c r="K31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L31" s="8" t="b">
+      <c r="L31" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1631,7 +1661,8 @@
       <c r="K32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L32" s="8" t="b">
+      <c r="L32" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1669,7 +1700,8 @@
       <c r="K33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L33" s="8" t="b">
+      <c r="L33" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1707,7 +1739,8 @@
       <c r="K34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L34" s="8" t="b">
+      <c r="L34" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1745,7 +1778,8 @@
       <c r="K35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L35" s="8" t="b">
+      <c r="L35" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1783,7 +1817,8 @@
       <c r="K36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L36" s="8" t="b">
+      <c r="L36" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1856,8 @@
       <c r="K37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L37" s="8" t="b">
+      <c r="L37" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1859,7 +1895,8 @@
       <c r="K38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L38" s="8" t="b">
+      <c r="L38" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1897,7 +1934,8 @@
       <c r="K39" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L39" s="8" t="b">
+      <c r="L39" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1935,7 +1973,8 @@
       <c r="K40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L40" s="8" t="b">
+      <c r="L40" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -1973,7 +2012,8 @@
       <c r="K41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L41" s="8" t="b">
+      <c r="L41" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2011,7 +2051,8 @@
       <c r="K42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="8" t="b">
+      <c r="L42" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2049,7 +2090,8 @@
       <c r="K43" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L43" s="8" t="b">
+      <c r="L43" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2087,7 +2129,8 @@
       <c r="K44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="8" t="b">
+      <c r="L44" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2125,7 +2168,8 @@
       <c r="K45" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L45" s="8" t="b">
+      <c r="L45" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2163,7 +2207,8 @@
       <c r="K46" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L46" s="8" t="b">
+      <c r="L46" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2201,7 +2246,8 @@
       <c r="K47" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L47" s="8" t="b">
+      <c r="L47" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2239,7 +2285,8 @@
       <c r="K48" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L48" s="8" t="b">
+      <c r="L48" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -2277,7 +2324,8 @@
       <c r="K49" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L49" s="8" t="b">
+      <c r="L49" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>